<commit_message>
Code rearranged to make it more readable
</commit_message>
<xml_diff>
--- a/YA Exhibition Summary.xlsx
+++ b/YA Exhibition Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnbar\Dropbox\OAS\OAS_Finances_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48279542-E04D-41FD-A65C-96AAB8E3F601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF6F716-A8E5-48F9-9D6E-F65600315730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="4192" windowWidth="16200" windowHeight="9308" xr2:uid="{8B5454ED-CD59-4425-961A-C9024C5F70A9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{8B5454ED-CD59-4425-961A-C9024C5F70A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Prizes</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>£200 refund due</t>
-  </si>
-  <si>
-    <t>One prize still to be claimed</t>
   </si>
 </sst>
 </file>
@@ -492,7 +489,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -531,10 +528,7 @@
         <v>-1000</v>
       </c>
       <c r="C4" s="3">
-        <v>-300</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
+        <v>-400</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -545,7 +539,7 @@
         <v>-1250</v>
       </c>
       <c r="C5" s="3">
-        <v>-638.4</v>
+        <v>-1126.8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -607,7 +601,7 @@
       </c>
       <c r="C11" s="4">
         <f>SUM(C3:C10)</f>
-        <v>-1536.44</v>
+        <v>-2124.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>